<commit_message>
Add graph for deflate
</commit_message>
<xml_diff>
--- a/clasp-report.xlsx
+++ b/clasp-report.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karstenpoeck/kpoeck.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{726E9240-21A7-E14B-BACC-B9DA62BEADC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66C0283-7AD0-534E-AE91-CA67DCF276E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="960" windowWidth="27840" windowHeight="16180"/>
+    <workbookView xWindow="680" yWindow="940" windowWidth="27840" windowHeight="16180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
-    <sheet name="compiler" sheetId="5" r:id="rId2"/>
-    <sheet name="arrays" sheetId="4" r:id="rId3"/>
-    <sheet name="crc40" sheetId="2" r:id="rId4"/>
-    <sheet name="boyer etc" sheetId="3" r:id="rId5"/>
+    <sheet name="deflate" sheetId="6" r:id="rId2"/>
+    <sheet name="compiler" sheetId="5" r:id="rId3"/>
+    <sheet name="arrays" sheetId="4" r:id="rId4"/>
+    <sheet name="crc40" sheetId="2" r:id="rId5"/>
+    <sheet name="boyer etc" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -512,7 +513,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1128,6 +1129,620 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>report!$A$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DEFLATE-FILE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>report!$B$3:$BD$3</c:f>
+              <c:strCache>
+                <c:ptCount val="55"/>
+                <c:pt idx="0">
+                  <c:v>Best</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20180628T0046</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20180701T1431</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20180625T2248</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20180628T2033</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20180628T2324</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20180630T1406</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20180701T1354</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20180703T0052</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20180710T2110</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20180710T2110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20180714T1124</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20180731T2329</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20180901T2325</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20180901T2325</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20180921T0700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20181216T2032</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20190414T0203</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20190427T2035</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20190507T0240</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20190430T2032</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20190507T0146</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20190502T0128</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20190505T0237</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>20190512T1523</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20190512T1523</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20190512T1523</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20190512T1126</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20190519T2132</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20190521T1245</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>20190601T1832</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20190608T1654</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20190610T1418</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20190610T1345</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20190615T1430</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20190615T1709</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20190615T1709</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20190616T1559</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>20190627T1035</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>20190705T2236</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20190720T1959</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20190720T1959</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20191208T1842</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20200104T1103</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>20200104T1344</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>20200218T2118</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20200219T0159</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>20200220T1822</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20200220T1822</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20200221T1811</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>20200221T1811</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>20200220T0757</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>20200219T2208</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>20200218T1436</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>20200221T2022</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>report!$B$52:$BD$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="55"/>
+                <c:pt idx="0">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6300000000000008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.48</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.86</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.88</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.26</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.49</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.69</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.71</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.58</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.58</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.23</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.56</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A195-FB4B-9A59-46733B321FB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="588416239"/>
+        <c:axId val="553756863"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="588416239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="553756863"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="553756863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588416239"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>report!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1687,7 +2302,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -3116,7 +3731,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -3730,7 +4345,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -5290,6 +5905,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7341,7 +7996,553 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D243DA2-1843-B44A-98C3-3EB224EC1028}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7384,7 +8585,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7427,7 +8628,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7470,7 +8671,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7809,11 +9010,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" activeCellId="1" sqref="A4:XFD4 A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" activeCellId="1" sqref="A52:XFD52 A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18949,7 +20150,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8740682-5EC2-3449-AFED-DA46CAAC0A49}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18963,21 +20179,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18990,7 +20193,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>